<commit_message>
made define in CharacterHandler
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,18 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>определение</t>
   </si>
   <si>
     <t>пример использования</t>
-  </si>
-  <si>
-    <t>bg [путь до файла без расширения]</t>
-  </si>
-  <si>
-    <t>bg gg_room</t>
   </si>
   <si>
     <t>изменение фонового изображения</t>
@@ -50,26 +44,930 @@
     <t>bg-color [0 - 255] [0 - 255] [0 - 255]</t>
   </si>
   <si>
-    <t>цвет в формате rgb, в примере - светло-голубой, который накладывается на фоновое изображение</t>
-  </si>
-  <si>
     <t>fg-color [0 - 255] [0 - 255] [0 - 255] [0 - 255]</t>
   </si>
   <si>
-    <t>bg gg_room bg-color 171 201 255</t>
+    <t>создание объектов персонажей для диалога</t>
   </si>
   <si>
-    <t>bg gg_room fg-color 171 201 255 100</t>
+    <t>bg [относительный путь до файла без расширения без кавычек]</t>
   </si>
   <si>
-    <t>цвет в формате rgba, в примере - полупрозрачный светло-голубой, который накладывается на все, что видит пользователь (фоновое изображение, спрайты персонажей и прочие объекты в диалоговом окне, кроме элементов интерфейса)</t>
+    <t>define [имя переменной персонажа] [относительный путь до папки без кавычек]</t>
+  </si>
+  <si>
+    <t>define aldv everlasting_suction/alice_dvachevskaya</t>
+  </si>
+  <si>
+    <t>bg alloto_location/first</t>
+  </si>
+  <si>
+    <t>bg alloto_location/first bg-color 171 201 255</t>
+  </si>
+  <si>
+    <t>bg alloto_location/first fg-color 171 201 255 100</t>
+  </si>
+  <si>
+    <t>bg alloto_location/first bg-color 171 201 255 fg-color 12 31 200 50</t>
+  </si>
+  <si>
+    <t>отображение картинок персонажей в диалоге</t>
+  </si>
+  <si>
+    <t>ВАЖНОЕ</t>
+  </si>
+  <si>
+    <t>картинки заднего фона должны иметь разрешение 16:9, например 1920 на 1080</t>
+  </si>
+  <si>
+    <t>спрайты персонажей должны иметь высоту 1080 пикселей и любую ширину
+в случае, если персонаж должен быть низким (если продолжать аналогию с БЛ, то Ульяна), высоту все равно стоит оставить 1080, а персонажа стоит расположить горизонтально по середине и вертикально снизу, так чтобы он ступнями "стоял" на нижней границе, а сверху оставить пустое место
+ну и вообще распологать персонажей стоит горизонтально по середине и вертикально снизу</t>
+  </si>
+  <si>
+    <t>show [имя переменной персонажа] [название эмоции]</t>
+  </si>
+  <si>
+    <t>show aldv smile</t>
+  </si>
+  <si>
+    <t>чтобы использовать это, сначала надо сделать define</t>
+  </si>
+  <si>
+    <t>atHorizontal [left / midleft / middle / midright / right]</t>
+  </si>
+  <si>
+    <r>
+      <t>так же можно передавать</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> сразу 2 аргумента</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+в данном случае и</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bg-color </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fg-color</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в дальнейшем все прочие аргументы</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> у всех команд можно будет передавать одновременно</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>цвет в формате</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rgb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+в примере - светло-голубой, который накладывается на фоновое изображение</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">цвет в формате </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rgba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>в примере - полупрозрачный светло-голубой</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, который накладывается на все, что видит пользователь (фоновое изображение, спрайты персонажей и прочие объекты в диалоговом окне, кроме элементов интерфейса)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">отображает персонажа в диалоге с эмоцией и распологает его по горизонтали следующим образом:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - слева
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midleft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "слева" и "по центру"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>middle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - по центру
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midright</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "справа" и "по центру"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - справа
+строка в примере расположит злую Алису между "справа" и "посередине"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВНИМАНИЕ!!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+файлы сохраняются в отдельно отведенной им папке проекта и путь надо писать </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>относительно нее</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (это папка Assets/Resources/backgrounds). 
+Допустим, наш файл - "Assets/Resources/backgrounds/alloto_location/first.png", 
+тогда мы пишем </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"alloto_location/first"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 
+Также в именах вложенных папок и самих файлов</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> не должно быть пробелов</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в данном случае в alloto_location </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>пробел заменен на _</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Файлы типа</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> png, jpg (jpeg)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>в данном случае все спрайты персонажей хранятся в одной общей папке (это папка Assets/Resources/charactersImages), 
+в таком случае, в примере в папке</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> charactersImages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> хранится папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>everlasting_suction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (на самом деле ее там нет), 
+в которой хранится папка</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> alice_dvachevskaya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+в которой хранятся спрайты(картинки) разных эмоций моей вайфу топ 1 (дада, вот до чего доводит кхд и сидение за компом по 10 часов в сутки). 
+ПО СУТИ ПЕРСОНАЖ С ТОЧКИ ЗРЕНИЯ ДИАЛОГА - ЭТО ПАПКА СО СПРАЙТАМИ ЭМОЦИЙ ПЕРСОНАЖА(ФАЙЛАМИ PNG JPG)
+например в папке alice_dvachevskaya могут быть следующие файлы:
+1) rage.png (тут будет картинка злой Алисочки)
+2) norm.png (тут будет картинка нормальной Алисочки)
+3) smile.png (тут будет картинка улыбающейся Алисочки)
+ в дальнейшем названия эмоций будут браться из имен этих файлов (rage, norm, smile)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">отображает персонажа в диалоге с эмоцией
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+имя переменной персонажа</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - это то имя, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>которое вы задали в define</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в нашем случае это</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aldv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (см. пример использования define)
+строка из примера отобразит улыбающуюся Алису, то есть картинку smile.png (см. комментарии к define)</t>
+    </r>
+  </si>
+  <si>
+    <t>степень реализации (реализует все это Азим)</t>
+  </si>
+  <si>
+    <t>РЕАЛИЗОВАНО</t>
+  </si>
+  <si>
+    <t>НЕ ПРОТЕСТИРОВАНО</t>
+  </si>
+  <si>
+    <t>НЕ РЕАЛИЗОВАНО</t>
+  </si>
+  <si>
+    <t>atVertical [top / midtop / middle / midbottom / bottom]</t>
+  </si>
+  <si>
+    <t>show aldv rage atHorizontal midright</t>
+  </si>
+  <si>
+    <t>show aldv norm atVertical top</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">отображает персонажа в диалоге с эмоцией и распологает его по вертикали следующим образом:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>top</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - сверху
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midtop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "сверху" и "по центру"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>middle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - по центру
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midbottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "снизу" и "по центру"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bottom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - снизу
+строка в примере расположит нормальную Алису сверху</t>
+    </r>
+  </si>
+  <si>
+    <t>atDistance [front / midfront / middle / midback / back]</t>
+  </si>
+  <si>
+    <t>show aldv smile atDistance middle</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">отображает персонажа в диалоге с эмоцией и распологает его по дальности следующим образом:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>front</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - близко
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midfront</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "близко" и "средне"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>middle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - средне (видно примерно половину спрайта)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>midback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - между "в полный рост" и "средне"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>back</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - в полный рост (типо так, что видно весь спрайт)
+строка в примере расположит нормальную Алису сверху</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +976,66 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,10 +1047,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -107,9 +1060,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,8 +1359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P594"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,23 +1371,29 @@
     <col min="3" max="3" width="64.42578125" customWidth="1"/>
     <col min="4" max="4" width="69.140625" customWidth="1"/>
     <col min="5" max="5" width="51.140625" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -427,20 +1404,26 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:16" ht="210" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -451,20 +1434,22 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -475,20 +1460,22 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -499,14 +1486,20 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -517,7 +1510,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -535,14 +1528,26 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:16" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -553,14 +1558,26 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -571,14 +1588,22 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -589,14 +1614,22 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -607,14 +1640,22 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -11121,5 +12162,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made default show character
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>определение</t>
   </si>
@@ -690,9 +690,6 @@
     <t>РЕАЛИЗОВАНО</t>
   </si>
   <si>
-    <t>НЕ ПРОТЕСТИРОВАНО</t>
-  </si>
-  <si>
     <t>НЕ РЕАЛИЗОВАНО</t>
   </si>
   <si>
@@ -964,6 +961,154 @@
   </si>
   <si>
     <t>еще надо добавить музыку</t>
+  </si>
+  <si>
+    <t>добавить wait</t>
+  </si>
+  <si>
+    <t>добавить скрыватель диалогового поля и тряситель экрана(для эффектов тряски)</t>
+  </si>
+  <si>
+    <t>layer [число, большее или равное нулю]</t>
+  </si>
+  <si>
+    <t>define aldv2 everlasting_suction/alice_dvachevskaya
+show aldv smile atDistance middle layer 1
+show aldv2 rage atDistance midfront layer 0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">так же стоит обратить внимание на то, что </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>atDistance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>layer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - это не одно и то же:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>atDistance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - влияет на дальность персонажа от нас
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>layer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - определяет на какой "срез" мы поместим персонажа</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">картинки персонажей, имеющие меньший </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>layer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (уровень прорисовки) отрисовываются поверх тех, что имеют больший уровень. 
+Можно представить, что пространство под экраном поделено на "срезы" и нулевой срез самый ближний, первый - за ним, второй - за первым и т д
+строки в примере делают следующее:
+  1. создание новой переменной Алисы
+  2. отрисовка первой алисы на средней дистанции на 1 уровне
+  3. отрисовка второй Алисы на 0 уровне на более ближней дистанции
+в итоге на экране будет следующее:
+две Алисы, первая будет дальше и за спиной у второй, а вторая - ближе и поверх первой</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1364,7 +1509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,6 +1521,7 @@
     <col min="5" max="5" width="51.140625" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
     <col min="7" max="7" width="41.85546875" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -1549,7 +1695,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1"/>
@@ -1579,7 +1725,7 @@
         <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1"/>
@@ -1598,14 +1744,14 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
@@ -1621,22 +1767,24 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1647,40 +1795,54 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="270" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1726,9 +1888,6 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1746,7 +1905,6 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1764,7 +1922,6 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>

</xml_diff>

<commit_message>
Show character handler completed
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>определение</t>
   </si>
@@ -78,11 +78,6 @@
   </si>
   <si>
     <t>картинки заднего фона должны иметь разрешение 16:9, например 1920 на 1080</t>
-  </si>
-  <si>
-    <t>спрайты персонажей должны иметь высоту 1080 пикселей и любую ширину
-в случае, если персонаж должен быть низким (если продолжать аналогию с БЛ, то Ульяна), высоту все равно стоит оставить 1080, а персонажа стоит расположить горизонтально по середине и вертикально снизу, так чтобы он ступнями "стоял" на нижней границе, а сверху оставить пустое место
-ну и вообще распологать персонажей стоит горизонтально по середине и вертикально снизу</t>
   </si>
   <si>
     <t>show [имя переменной персонажа] [название эмоции]</t>
@@ -969,9 +964,6 @@
     <t>добавить скрыватель диалогового поля и тряситель экрана(для эффектов тряски)</t>
   </si>
   <si>
-    <t>layer [число, большее или равное нулю]</t>
-  </si>
-  <si>
     <t>define aldv2 everlasting_suction/alice_dvachevskaya
 show aldv smile atDistance middle layer 1
 show aldv2 rage atDistance midfront layer 0</t>
@@ -1076,6 +1068,202 @@
     </r>
   </si>
   <si>
+    <t>удаление персонажа с экрана</t>
+  </si>
+  <si>
+    <t>hide [имя переменной]</t>
+  </si>
+  <si>
+    <t>hide aldv</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">картинка персонажа просто пропадет с экрана, но сама переменная останется и позже можно будет снова отрисовать этого персонажа, просто прописав </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">show
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">например, в этом случае, чтобы снова отрисовать Алису нужно прописать:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show aldv</t>
+    </r>
+  </si>
+  <si>
+    <t>удаление переменной персонажа</t>
+  </si>
+  <si>
+    <t>destroy [имя переменной]</t>
+  </si>
+  <si>
+    <t>destroy aldv</t>
+  </si>
+  <si>
+    <t>картинка персонажа пропадет с экрана, и переменная, по которой вы к персонажу обращались так же уничтожится</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">при использовании </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">hide </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">персонаж просто "прячется"
+а при использовании </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">destroy </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">уничтожается
+настоятельно рекомендуется использовать </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>destroy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> по окончанию каждого конечного диалога (диалога, который не имеет вариантов ответа, запускающих последующие диалоги)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">спрайты персонажей должны иметь высоту 1080 пикселей и любую ширину
+в случае, если персонаж должен быть низким (если продолжать аналогию с БЛ, то Ульяна), высоту все равно стоит оставить 1080, а персонажа стоит расположить горизонтально по середине и вертикально снизу, так чтобы он ступнями "стоял" на нижней границе, а сверху оставить пустое место
+ну и вообще распологать персонажей стоит горизонтально по середине и вертикально снизу
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ВНИМАНИЕ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">переменные персонажей не удаляются автоматически, поэтому, если вы задефайнили персонажа в одном диалоге и потом из этого диалога за счет вариантов ответа вы запускаете новый диалог, при этом </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">НЕ ЗАКРЫВАЯ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>диалоговое окно, то переменные будут актуальны, и персонажи, при переходе на следующий диалог останутся в тех же положениях, что и были до перехода</t>
+    </r>
+  </si>
+  <si>
+    <t>layer [0 - 100]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">картинки персонажей, имеющие больший </t>
     </r>
@@ -1100,7 +1288,53 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (уровень прорисовки) отрисовываются поверх тех, что имеют меньший уровень. 
+      <t xml:space="preserve"> (уровень прорисовки) отрисовываются поверх тех, что имеют меньший уровень. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">layer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">может быть </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>от 0 до 100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Можно представить, что пространство под экраном поделено на "срезы" и нулевой срез  - самый дальний, первый - перед ним, второй - перед первым и т д
 строки в примере делают следующее:
   1. создание новой переменной Алисы (</t>
@@ -1635,8 +1869,8 @@
   <dimension ref="A1:P594"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1902,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
@@ -1692,13 +1926,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
@@ -1720,11 +1954,11 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
@@ -1746,11 +1980,11 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="1"/>
@@ -1770,11 +2004,11 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="1"/>
@@ -1816,13 +2050,13 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1"/>
@@ -1839,20 +2073,20 @@
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="1"/>
@@ -1868,17 +2102,17 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
@@ -1894,23 +2128,23 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1922,23 +2156,23 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1946,29 +2180,29 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="285" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="300" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1994,14 +2228,24 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2012,13 +2256,25 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+    <row r="15" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>

</xml_diff>

<commit_message>
made parametr with to add animations in Show() in character handler
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>определение</t>
   </si>
@@ -1471,12 +1471,77 @@
       <t>aldv</t>
     </r>
   </si>
+  <si>
+    <t>with [имя_анимации] [длительность_в_секундах]</t>
+  </si>
+  <si>
+    <t>show aldv smile atDistance midfront atHorizontal right with fade 3,14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СООБЩЕНИЕ САМОМУ СЕБЕ
+Азим, сделай анимашек побольше </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">пока что доступны следующие виды анимаций:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">fade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- постепенное появление от полностью прозрачного до непрозрачного
+в дальнейшем этот список будет пополняться
+длительность может быть дробным числом, может быть меньше 1 (0,5 например), и дробная часть пишется через </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ЗАПЯТУЮ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">в приведенном примере Алиса будет постепенно появлятся на протяжении 3,14 секунды на средне-ближнем расстоянии справа </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1528,8 +1593,25 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1546,6 +1628,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1556,12 +1643,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1584,8 +1672,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="2" builtinId="27"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26"/>
@@ -1869,8 +1961,8 @@
   <dimension ref="A1:P594"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,25 +2131,6 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -2068,22 +2141,22 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>15</v>
+    <row r="8" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>30</v>
@@ -2098,21 +2171,25 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="165" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>21</v>
+    <row r="9" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="1"/>
@@ -2124,21 +2201,21 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="1"/>
@@ -2152,21 +2229,21 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="1"/>
@@ -2180,23 +2257,21 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="300" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="1"/>
@@ -2210,14 +2285,24 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="300" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -2228,23 +2313,23 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="120" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>44</v>
+    <row r="14" spans="1:16" ht="195" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>56</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="1"/>
@@ -2256,25 +2341,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="150" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>31</v>
-      </c>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2285,13 +2352,24 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+    <row r="16" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2302,13 +2380,25 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+    <row r="17" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>

</xml_diff>

<commit_message>
made Waiter and WaitHandler (they works correctly)
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>определение</t>
   </si>
@@ -1672,6 +1672,264 @@
         <scheme val="minor"/>
       </rPr>
       <t>в примере картинка будет исчезать на протяжении 1,4 секунды, после чего, вместо заднего фона на экране останется черный экран</t>
+    </r>
+  </si>
+  <si>
+    <t>приостановить выполнение сервисных реплик на время</t>
+  </si>
+  <si>
+    <t>wait [время в секундах]</t>
+  </si>
+  <si>
+    <t>show aldv with fade 0,5
+wait 0,5
+show lena with fade 1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">помимо сервисных реплик </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wait</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> так же стопорит обычные реплики, 
+то есть при использовании</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wait не получится перейти на следующую реплику, пока wait ждет</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (кнопка просто не будет реагировать), и после истечения времени </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wait</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, снова </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>можно будет перейти</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C0006"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на следующую реплику</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>в примере произойдет следующее:
+Алиса начнет появляться с анимацией</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> на протяжении 0,5 секунд и</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> после окончания этой анимации</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> начнет появляться Лена (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wait </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">будет ждать 0,5 секунд, а это как раз длительность анимации Алисы)
+в случае если будет написано:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">show aldv with fade 0,5
+show lena with fade 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">то Алиса и Лена </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>начнут появляться одновременно</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+в общем штука полезна, если вы хотите </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>настроить очередность появлений</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> персонажей, смены бэкграунда, цвета и т д и т п</t>
     </r>
   </si>
 </sst>
@@ -2098,9 +2356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P594"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2644,14 +2902,26 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:16" ht="255" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>

</xml_diff>

<commit_message>
started refactoring background handler
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -2357,8 +2357,8 @@
   <dimension ref="A1:P594"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2562,52 +2562,29 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L8" s="2"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
+    <row r="9" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>29</v>
@@ -2622,45 +2599,47 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="165" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>21</v>
+    <row r="10" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
@@ -2670,7 +2649,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="1"/>
@@ -2678,17 +2657,17 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
@@ -2698,7 +2677,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="2"/>
       <c r="M12" s="1"/>
@@ -2706,48 +2685,48 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="300" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>41</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="300" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>56</v>
+      <c r="F14" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>29</v>
@@ -2762,14 +2741,24 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2798,24 +2787,14 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="120" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -2826,50 +2805,48 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="180" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
+    <row r="18" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>42</v>
       </c>
+      <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="150" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>46</v>
+    <row r="19" spans="1:16" ht="180" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>29</v>
@@ -2884,14 +2861,26 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+    <row r="20" spans="1:16" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2902,26 +2891,14 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="255" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>71</v>
-      </c>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2932,14 +2909,26 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+    <row r="22" spans="1:16" ht="255" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>

</xml_diff>

<commit_message>
started audio in dialogs
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t>определение</t>
   </si>
@@ -387,139 +387,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ВНИМАНИЕ!!!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-файлы сохраняются в отдельно отведенной им папке проекта и путь надо писать </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>относительно нее</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (это папка Assets/Resources/backgrounds). 
-Допустим, наш файл - "Assets/Resources/backgrounds/alloto_location/first.png", 
-тогда мы пишем </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"alloto_location/first"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. 
-Также в именах вложенных папок и самих файлов</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> не должно быть пробелов</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> в данном случае в alloto_location </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>пробел заменен на _</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Файлы типа</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> png, jpg (jpeg)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">отображает персонажа в диалоге с эмоцией
 </t>
     </r>
@@ -869,12 +736,6 @@
     </r>
   </si>
   <si>
-    <t>еще надо добавить музыку</t>
-  </si>
-  <si>
-    <t>добавить wait</t>
-  </si>
-  <si>
     <t>добавить скрыватель диалогового поля и тряситель экрана(для эффектов тряски)</t>
   </si>
   <si>
@@ -1517,89 +1378,6 @@
     <t>duration [время_смены_картинки] [время_смены_bg_color] [время_смены_fg_color]</t>
   </si>
   <si>
-    <r>
-      <t>в данном случае все спрайты персонажей хранятся в одной общей папке (это папка Assets/Resources/charactersImages), 
-в таком случае, в примере в папке</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> charactersImages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> хранится папка </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>everlasting_suction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (на самом деле ее там нет), 
-в которой хранится папка</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> alice_dvachevskaya</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 
-в которой хранятся спрайты(картинки) разных эмоций моей еот (дада, вот до чего доводит кхд и сидение за компом по 10 часов в сутки). 
-ПО СУТИ ПЕРСОНАЖ С ТОЧКИ ЗРЕНИЯ ДИАЛОГА - ЭТО ПАПКА СО СПРАЙТАМИ ЭМОЦИЙ ПЕРСОНАЖА(ФАЙЛАМИ PNG JPG)
-например в папке alice_dvachevskaya могут быть следующие файлы:
-1) rage.png (тут будет картинка злой Алисочки)
-2) norm.png (тут будет картинка нормальной Алисочки)
-3) smile.png (тут будет картинка улыбающейся Алисочки)
- в дальнейшем названия эмоций будут браться из имен этих файлов (rage, norm, smile)</t>
-    </r>
-  </si>
-  <si>
     <t>bg alloto_location/first bg-color 171 201 255 fg-color 12 31 200 50 duration 1,5 3 2,1</t>
   </si>
   <si>
@@ -1928,6 +1706,733 @@
       </rPr>
       <t xml:space="preserve"> персонажей, смены бэкграунда, цвета и т д и т п</t>
     </r>
+  </si>
+  <si>
+    <t>проигрывание музыки</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВНИМАНИЕ!!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+файлы сохраняются в отдельно отведенной им папке проекта и путь надо писать </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>относительно нее</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (это папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assets/Resources/backgrounds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">). 
+Допустим, наш файл - "Assets/Resources/backgrounds/alloto_location/first.png", 
+тогда мы пишем </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"alloto_location/first"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. 
+Также в именах вложенных папок и самих файлов</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> не должно быть пробелов</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в данном случае в alloto_location </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>пробел заменен на _</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Файлы типа</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> png, jpg (jpeg)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВНИМАНИЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+все спрайты персонажей хранятся в одной общей папке (это папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assets/Resources/charactersImages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), 
+в таком случае, в примере в папке</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> charactersImages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> хранится папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>everlasting_suction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (на самом деле ее там нет), 
+в которой хранится папка</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> alice_dvachevskaya</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+в которой хранятся спрайты(картинки) разных эмоций моей еот (дада, вот до чего доводит кхд и сидение за компом по 10 часов в сутки). 
+ПО СУТИ ПЕРСОНАЖ С ТОЧКИ ЗРЕНИЯ ДИАЛОГА - ЭТО ПАПКА СО СПРАЙТАМИ ЭМОЦИЙ ПЕРСОНАЖА(ФАЙЛАМИ PNG JPG)
+например в папке alice_dvachevskaya могут быть следующие файлы:
+1) rage.png (тут будет картинка злой Алисочки)
+2) norm.png (тут будет картинка нормальной Алисочки)
+3) smile.png (тут будет картинка улыбающейся Алисочки)
+ в дальнейшем названия эмоций будут браться из имен этих файлов (rage, norm, smile)</t>
+    </r>
+  </si>
+  <si>
+    <t>play [относительный путь до файла без расширения и кавычек] [имя источника звука]</t>
+  </si>
+  <si>
+    <t>play alice_theme/krutaya_muzyka alices_hlebych</t>
+  </si>
+  <si>
+    <t>НЕ РЕАЛИЗОВАНО</t>
+  </si>
+  <si>
+    <t>volume [0 - 100]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ВНИМАНИЕ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+все звуки хранятся в одной общей папке (это папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Assets/Resources/sounds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">), 
+в таком случае в папке </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Assets/Resources/sounds </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">хранится папка </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>alice_theme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> в которой хранится композиция </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">krutaya_muzyka.mp4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(ну у нее реально норм музыка)
+зачем </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>нужны источники звука</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">?
+допустим, у нас только один источник как бы "по умолчанию" и допустим, что нам надо врубить две композиции одновременно, но </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">нихера не выйдет, источник то один
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">в таком случае к нам </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">на помощь и приходят разные источники звука
+создавать источник не надо </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">в случае, если вы один раз написали новое, ранее не используемое имя источника, то источник </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">создастся сам автоматически и будет доступен для дальнейшего использования
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">в случае же, если вы использовали </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>какой-либо ранее использованный источник</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, то в случае, если на нем играется какая-либо композиция, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ее проигрывание прерывается и начинает играть та композиция, которая была передана источнику
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">громкость проигрывания композиции в процентах
+может быть дробным числом, дробная часть пишется через </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ЗАПЯТУЮ</t>
+    </r>
+  </si>
+  <si>
+    <t>play elektronik/gay_party another_source volume 70,3</t>
+  </si>
+  <si>
+    <t>loop</t>
+  </si>
+  <si>
+    <t>play alice_theme/krutaya_muzyka alices_hlebych volume 40 loop</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">зацикливает проигрывание, то есть при использовании </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">loop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">по окончанию композиции </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>она заиграет снова и так бесконечно…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Ну или пока вы не прервете проигрывание другим </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">play </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>на этот источник звука</t>
+    </r>
+  </si>
+  <si>
+    <t>изменение громкости источника</t>
+  </si>
+  <si>
+    <t>change-volume [имя источника] [громкость]</t>
+  </si>
+  <si>
+    <t>change-volume alices_hlebych 80</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">увеличивает громкость источника в процессе проигрывания
+в примере громкость источника </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>alices_hlebych</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, который из прошлого примера зациклен на </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">alice_theme/krutaya_muzyka </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>на громкости 40 повысит свою громкость до 80</t>
+    </r>
+  </si>
+  <si>
+    <t>ВАЖНО чтобы источник звука был известен (был ранее используем), иначе будет ошибка</t>
+  </si>
+  <si>
+    <t>остановить проигрывание музыки</t>
+  </si>
+  <si>
+    <t>stop [имя источника звука]</t>
+  </si>
+  <si>
+    <t>stop alices_hlebych</t>
+  </si>
+  <si>
+    <t>останавливает проигрывание музыки на каком либо источнике</t>
   </si>
 </sst>
 </file>
@@ -2353,9 +2858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P594"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2892,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
@@ -2411,13 +2916,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="1"/>
@@ -2443,7 +2948,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -2469,7 +2974,7 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2493,7 +2998,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2509,17 +3014,17 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2533,21 +3038,21 @@
     </row>
     <row r="7" spans="1:16" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2578,13 +3083,13 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2608,13 +3113,13 @@
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2633,21 +3138,19 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2658,24 +3161,22 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2686,23 +3187,23 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="1"/>
@@ -2714,19 +3215,19 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2742,19 +3243,19 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F15" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2804,21 +3305,21 @@
     </row>
     <row r="18" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -2834,19 +3335,19 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="1"/>
@@ -2860,23 +3361,23 @@
     </row>
     <row r="20" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="1"/>
@@ -2908,23 +3409,23 @@
     </row>
     <row r="22" spans="1:16" ht="255" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="1"/>
@@ -2954,14 +3455,24 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+    <row r="24" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2972,14 +3483,22 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2990,12 +3509,18 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -3026,14 +3551,26 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+    <row r="28" spans="1:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -3062,14 +3599,25 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+    <row r="30" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>

</xml_diff>

<commit_message>
made moving in dialogsystem, it is completed
</commit_message>
<xml_diff>
--- a/Assets/api.xlsx
+++ b/Assets/api.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>определение</t>
   </si>
@@ -2470,9 +2470,6 @@
   </si>
   <si>
     <t>чтобы использовать moving нужно, чтобы персонаж при этом был показан на экране</t>
-  </si>
-  <si>
-    <t>НЕ РЕАЛИЗОВАНО</t>
   </si>
 </sst>
 </file>
@@ -3319,8 +3316,8 @@
       <c r="F16" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>95</v>
+      <c r="G16" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>

</xml_diff>